<commit_message>
Bi-weekly presentation and update on code
</commit_message>
<xml_diff>
--- a/Project plan/statusOnWriting.xlsx
+++ b/Project plan/statusOnWriting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tobias/Google Drev/UNI/Master-Thesis-Fall-2020/Project plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E631F85-B789-5041-BA00-E66704F6B32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C87B25-5762-1445-89BE-B377326E6859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1440" windowWidth="27840" windowHeight="15820" xr2:uid="{24523555-627A-F141-A28E-F754F9854B55}"/>
+    <workbookView xWindow="960" yWindow="1060" windowWidth="27840" windowHeight="15820" xr2:uid="{24523555-627A-F141-A28E-F754F9854B55}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Section</t>
   </si>
@@ -48,6 +48,36 @@
   </si>
   <si>
     <t>Introduction</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Previous work</t>
+  </si>
+  <si>
+    <t>Method for MNIST</t>
+  </si>
+  <si>
+    <t>Results for MNIST</t>
+  </si>
+  <si>
+    <t>Method TBD</t>
+  </si>
+  <si>
+    <t>Results TBD</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Concolusion</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Preface</t>
   </si>
 </sst>
 </file>
@@ -72,6 +102,7 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -113,7 +144,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -127,7 +209,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -155,11 +237,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -175,7 +257,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
@@ -183,7 +265,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -259,7 +341,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -303,7 +385,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,7 +425,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE5BBA0E-C699-CF4D-BB84-9CAA58DEAE2C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -417,14 +499,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1101" name="Check Box 77" descr=" " hidden="1">
@@ -433,7 +520,7 @@
                   <a14:compatExt spid="_x0000_s1101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7511F51A-1C14-ED4D-9FDD-95CA8B40EFC0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -501,20 +588,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1102" name="Check Box 78" descr=" " hidden="1">
@@ -523,7 +615,7 @@
                   <a14:compatExt spid="_x0000_s1102"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{389C845A-B0A8-C044-B4DA-D48EE189DBC8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -591,20 +683,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1103" name="Check Box 79" descr=" " hidden="1">
@@ -613,7 +710,7 @@
                   <a14:compatExt spid="_x0000_s1103"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FFEB782-9869-3B4F-BDC7-6DB56C1F250D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -681,20 +778,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1104" name="Check Box 80" descr=" " hidden="1">
@@ -703,7 +805,7 @@
                   <a14:compatExt spid="_x0000_s1104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF30F927-7DCB-764E-B9A0-4AA11B7279BF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -771,20 +873,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1105" name="Check Box 81" descr=" " hidden="1">
@@ -793,7 +900,7 @@
                   <a14:compatExt spid="_x0000_s1105"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{046E35FE-0566-AB40-8778-10895C3B9F72}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000051040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -861,20 +968,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1106" name="Check Box 82" descr=" " hidden="1">
@@ -883,7 +995,7 @@
                   <a14:compatExt spid="_x0000_s1106"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C15F4F6-4E80-8448-9A7D-067950AB0496}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000052040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -951,20 +1063,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1107" name="Check Box 83" descr=" " hidden="1">
@@ -973,7 +1090,7 @@
                   <a14:compatExt spid="_x0000_s1107"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB179EA1-EC9E-054B-9A86-099ADD930200}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1041,20 +1158,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1108" name="Check Box 84" descr=" " hidden="1">
@@ -1063,7 +1185,7 @@
                   <a14:compatExt spid="_x0000_s1108"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10C7B6F5-4E1D-5740-9DCD-CC79406282EA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000054040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1131,20 +1253,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1109" name="Check Box 85" descr=" " hidden="1">
@@ -1153,7 +1280,7 @@
                   <a14:compatExt spid="_x0000_s1109"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A37005AE-92E4-754E-8F2F-3FBF0EC083BF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1221,20 +1348,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1110" name="Check Box 86" descr=" " hidden="1">
@@ -1243,7 +1375,7 @@
                   <a14:compatExt spid="_x0000_s1110"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DE1E51-8CF8-3D47-B9EB-E0DFCD7E41FC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1311,20 +1443,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1111" name="Check Box 87" descr=" " hidden="1">
@@ -1333,7 +1470,7 @@
                   <a14:compatExt spid="_x0000_s1111"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED54C602-11B9-D84C-96D2-189EBF081DDD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1401,20 +1538,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1112" name="Check Box 88" descr=" " hidden="1">
@@ -1423,7 +1565,7 @@
                   <a14:compatExt spid="_x0000_s1112"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49C03674-E4AB-5441-9DDB-8B541624DD90}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000058040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1491,20 +1633,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1113" name="Check Box 89" descr=" " hidden="1">
@@ -1513,7 +1660,7 @@
                   <a14:compatExt spid="_x0000_s1113"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{345B85E6-2C2D-074B-9E8C-F18DCD13DB45}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000059040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1581,20 +1728,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1114" name="Check Box 90" descr=" " hidden="1">
@@ -1603,7 +1755,7 @@
                   <a14:compatExt spid="_x0000_s1114"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC7B6F2-BED5-CE4C-8736-E8B121AFBBCD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1671,20 +1823,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1115" name="Check Box 91" descr=" " hidden="1">
@@ -1693,7 +1850,7 @@
                   <a14:compatExt spid="_x0000_s1115"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EA67BDF-1908-C241-9C5C-98D76C090A7C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1761,20 +1918,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1116" name="Check Box 92" descr=" " hidden="1">
@@ -1783,7 +1945,7 @@
                   <a14:compatExt spid="_x0000_s1116"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C493663E-D0E2-8140-86B4-F866ACBB7045}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1851,20 +2013,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1117" name="Check Box 93" descr=" " hidden="1">
@@ -1873,7 +2040,7 @@
                   <a14:compatExt spid="_x0000_s1117"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D883110E-CBA5-B244-906B-9F6A02065094}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1941,20 +2108,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1118" name="Check Box 94" descr=" " hidden="1">
@@ -1963,7 +2135,7 @@
                   <a14:compatExt spid="_x0000_s1118"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0FA8756-6355-7A4E-8941-A62CEBE85B70}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2031,20 +2203,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1119" name="Check Box 95" descr=" " hidden="1">
@@ -2053,7 +2230,7 @@
                   <a14:compatExt spid="_x0000_s1119"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9216FDED-403B-B140-9E07-6D628704D16D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2121,20 +2298,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1120" name="Check Box 96" descr=" " hidden="1">
@@ -2143,7 +2325,7 @@
                   <a14:compatExt spid="_x0000_s1120"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC704B5-B1C5-C74E-9F7A-AC75238A923A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2211,20 +2393,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1121" name="Check Box 97" descr=" " hidden="1">
@@ -2233,7 +2420,7 @@
                   <a14:compatExt spid="_x0000_s1121"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDCE0DD8-B969-B04A-97D4-2D0E01FE6CD0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2301,20 +2488,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1122" name="Check Box 98" descr=" " hidden="1">
@@ -2323,7 +2515,7 @@
                   <a14:compatExt spid="_x0000_s1122"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA151369-D3E3-F14A-BCBE-8F3650ED742C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2391,20 +2583,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1123" name="Check Box 99" descr=" " hidden="1">
@@ -2413,7 +2610,7 @@
                   <a14:compatExt spid="_x0000_s1123"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D264CF1-10B1-F449-B3E9-B0D82486E981}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2481,20 +2678,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1124" name="Check Box 100" descr=" " hidden="1">
@@ -2503,7 +2705,7 @@
                   <a14:compatExt spid="_x0000_s1124"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C6530A2-D688-F045-A9FC-632280E7BC2E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000064040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2571,20 +2773,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1125" name="Check Box 101" descr=" " hidden="1">
@@ -2593,7 +2800,7 @@
                   <a14:compatExt spid="_x0000_s1125"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F26736FE-71D6-A943-A1BA-8A8B7811E084}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2661,20 +2868,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1126" name="Check Box 102" descr=" " hidden="1">
@@ -2683,7 +2895,7 @@
                   <a14:compatExt spid="_x0000_s1126"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{713F9962-1550-7C49-8D2A-09F54148ADE1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000066040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2751,20 +2963,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1127" name="Check Box 103" descr=" " hidden="1">
@@ -2773,7 +2990,7 @@
                   <a14:compatExt spid="_x0000_s1127"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C80F03CE-0B38-8E40-B73B-2A991E71A8DC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000067040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2841,20 +3058,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1128" name="Check Box 104" descr=" " hidden="1">
@@ -2863,7 +3085,7 @@
                   <a14:compatExt spid="_x0000_s1128"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B04F87-E0FF-AD4D-9325-77F4A05E3FA9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000068040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2931,20 +3153,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1129" name="Check Box 105" descr=" " hidden="1">
@@ -2953,7 +3180,7 @@
                   <a14:compatExt spid="_x0000_s1129"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2BADA49-19BE-6A44-9B2E-D81E85655878}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000069040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3021,20 +3248,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1130" name="Check Box 106" descr=" " hidden="1">
@@ -3043,7 +3275,7 @@
                   <a14:compatExt spid="_x0000_s1130"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A399854C-381D-BB4E-B13D-76F668C0DA98}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3111,20 +3343,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1131" name="Check Box 107" descr=" " hidden="1">
@@ -3133,7 +3370,7 @@
                   <a14:compatExt spid="_x0000_s1131"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E0DA8A2-73C2-7E4C-8DCD-1B257CF03FC9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3201,20 +3438,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1132" name="Check Box 108" descr=" " hidden="1">
@@ -3223,7 +3465,7 @@
                   <a14:compatExt spid="_x0000_s1132"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{490ADFB0-7AC0-394D-8D1D-8DE324E7AE19}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3291,20 +3533,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1133" name="Check Box 109" descr=" " hidden="1">
@@ -3313,7 +3560,7 @@
                   <a14:compatExt spid="_x0000_s1133"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5640DAC5-C241-1F43-AACB-9937FB87A668}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3381,20 +3628,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1134" name="Check Box 110" descr=" " hidden="1">
@@ -3403,7 +3655,7 @@
                   <a14:compatExt spid="_x0000_s1134"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CC8C19F-C849-AB41-AEBA-4A5D0B2A8A23}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3471,20 +3723,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1135" name="Check Box 111" descr=" " hidden="1">
@@ -3493,7 +3750,7 @@
                   <a14:compatExt spid="_x0000_s1135"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E50E74-1066-9147-AD12-01058521A642}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3561,20 +3818,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1136" name="Check Box 112" descr=" " hidden="1">
@@ -3583,7 +3845,7 @@
                   <a14:compatExt spid="_x0000_s1136"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E98458F9-87C2-DC43-9466-1B430F431251}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000070040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3651,20 +3913,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1137" name="Check Box 113" descr=" " hidden="1">
@@ -3673,7 +3940,7 @@
                   <a14:compatExt spid="_x0000_s1137"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B652FDE2-E33E-2A47-9820-364D3DB7E07B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000071040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3741,20 +4008,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1138" name="Check Box 114" descr=" " hidden="1">
@@ -3763,7 +4035,7 @@
                   <a14:compatExt spid="_x0000_s1138"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACA741F-6554-2B47-8252-3A865138B051}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3831,20 +4103,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1139" name="Check Box 115" descr=" " hidden="1">
@@ -3853,7 +4130,7 @@
                   <a14:compatExt spid="_x0000_s1139"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F02A9A7-6505-4E4A-9F2B-30A4E2BF00C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000073040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3921,20 +4198,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1140" name="Check Box 116" descr=" " hidden="1">
@@ -3943,7 +4225,7 @@
                   <a14:compatExt spid="_x0000_s1140"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81664D94-7C4A-AE4D-8E88-A1051B91C6B7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000074040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4011,20 +4293,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1141" name="Check Box 117" descr=" " hidden="1">
@@ -4033,7 +4320,7 @@
                   <a14:compatExt spid="_x0000_s1141"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E461C173-3774-D746-BB00-8BDAAEA3D361}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4101,20 +4388,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1142" name="Check Box 118" descr=" " hidden="1">
@@ -4123,7 +4415,7 @@
                   <a14:compatExt spid="_x0000_s1142"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC3905E-87D3-1C44-AFAF-BFFB346866D5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4191,20 +4483,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1143" name="Check Box 119" descr=" " hidden="1">
@@ -4213,7 +4510,7 @@
                   <a14:compatExt spid="_x0000_s1143"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{141967E3-5C97-B44B-8FCF-AB4D4FEAF2C3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000077040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4281,20 +4578,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1144" name="Check Box 120" descr=" " hidden="1">
@@ -4303,7 +4605,7 @@
                   <a14:compatExt spid="_x0000_s1144"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A61151D-4DF0-E74E-836D-7C471040FDAC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000078040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4371,20 +4673,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1145" name="Check Box 121" descr=" " hidden="1">
@@ -4393,7 +4700,7 @@
                   <a14:compatExt spid="_x0000_s1145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C675B33-2F73-2249-A688-1D711C336343}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000079040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4461,20 +4768,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1146" name="Check Box 122" descr=" " hidden="1">
@@ -4483,7 +4795,7 @@
                   <a14:compatExt spid="_x0000_s1146"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84BE02E8-3F2F-184C-9F61-DE25605A464E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4551,20 +4863,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>292100</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="279400" cy="381000"/>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1147" name="Check Box 123" descr=" " hidden="1">
@@ -4573,7 +4890,7 @@
                   <a14:compatExt spid="_x0000_s1147"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2D3281C-32FB-7F44-B5C3-BCAD479CE7A2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4641,7 +4958,7 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -4945,10 +5262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FAC869-5C3A-0944-80FC-52DD32ECCF2F}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4972,11 +5289,66 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1"/>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"True"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>